<commit_message>
end dijkstra algorithm implementation
</commit_message>
<xml_diff>
--- a/rapport/Classeur1.xlsx
+++ b/rapport/Classeur1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33610\C\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\code_CPP\theorie_graph\TP3-theo-graph\rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3EE0877-67FE-445C-B586-5A5C4D122251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9EDD05-3D14-45F1-A4AB-9300177B8279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{96DC5565-B0D4-4BB4-BAEA-97FBC111761F}"/>
+    <workbookView xWindow="15480" yWindow="15" windowWidth="12015" windowHeight="11505" xr2:uid="{96DC5565-B0D4-4BB4-BAEA-97FBC111761F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>SOMMET</t>
   </si>
@@ -121,9 +119,6 @@
     <t>0 14 7</t>
   </si>
   <si>
-    <t>0 11  13</t>
-  </si>
-  <si>
     <t>0 9 12</t>
   </si>
   <si>
@@ -133,10 +128,16 @@
     <t>1 9 6</t>
   </si>
   <si>
-    <t>1 11 13</t>
-  </si>
-  <si>
     <t>ETAPE</t>
+  </si>
+  <si>
+    <t>0 16 10</t>
+  </si>
+  <si>
+    <t>1 16 10</t>
+  </si>
+  <si>
+    <t>1 14 7</t>
   </si>
 </sst>
 </file>
@@ -174,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +209,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -303,6 +310,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -621,16 +631,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A2069CE-5C0C-476D-8980-02AC72B5D3EB}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -680,9 +690,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
@@ -700,7 +710,7 @@
       <c r="O2" s="8"/>
       <c r="P2" s="9"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -750,7 +760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -778,7 +788,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -804,7 +814,7 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -828,7 +838,7 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -852,7 +862,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -878,7 +888,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -900,7 +910,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -922,7 +932,7 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -950,7 +960,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -969,11 +979,11 @@
         <v>23</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -997,7 +1007,7 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -1021,7 +1031,7 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>12</v>
       </c>
@@ -1036,16 +1046,14 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="M15" s="10"/>
       <c r="N15" s="2"/>
       <c r="O15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P15" s="2"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -1064,10 +1072,10 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -1081,15 +1089,17 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="3" t="s">
+      <c r="L17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -1103,10 +1113,10 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -1122,6 +1132,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010049126D499BD5B840A5F6C0C3100F82EB" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="ee9e5b618ba35ea57394a7455918e9e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c750ebf5-1ef7-4cb6-bfbe-a13c905b81ec" xmlns:ns4="e84b4fb9-6979-42b0-8600-029ef793f30b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74c90eed5f07ed1304c5c1e77916c2cf" ns3:_="" ns4:_="">
     <xsd:import namespace="c750ebf5-1ef7-4cb6-bfbe-a13c905b81ec"/>
@@ -1310,22 +1335,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58772FBB-195A-49D7-B590-099E86F64DE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c750ebf5-1ef7-4cb6-bfbe-a13c905b81ec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e84b4fb9-6979-42b0-8600-029ef793f30b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B21E3017-A437-43EE-96C4-3FAE3540B67A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD007D37-8D5F-406B-B07C-735CFF483BE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1342,29 +1377,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B21E3017-A437-43EE-96C4-3FAE3540B67A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58772FBB-195A-49D7-B590-099E86F64DE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c750ebf5-1ef7-4cb6-bfbe-a13c905b81ec"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e84b4fb9-6979-42b0-8600-029ef793f30b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>